<commit_message>
V19. Se agrega el código en los modelos CNN-1D, el cual que permite registrar las métricas en cada repetición del experimento.
</commit_message>
<xml_diff>
--- a/modelos_CNN_1D/modelo2/resultados_iteraciones/resultados.xlsx
+++ b/modelos_CNN_1D/modelo2/resultados_iteraciones/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,54 @@
         <v>0.9137499928474426</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.2639766931533813</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9125000238418579</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.2397506684064865</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.9262499809265137</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.3285242021083832</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8862500190734863</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.317320704460144</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.887499988079071</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.3031081259250641</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8987500071525574</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.2830060124397278</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.9162499904632568</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>